<commit_message>
added notes on subnational weighted averaging
</commit_message>
<xml_diff>
--- a/pre_processing/lsff_project/data_prep/LSFF_data_prep_version0_notes.xlsx
+++ b/pre_processing/lsff_project/data_prep/LSFF_data_prep_version0_notes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Country</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>Kano is the capital city of kano state, and the second-largest city in nigeria. Lagos is the post populous city in Nigeria.</t>
+  </si>
+  <si>
+    <t>Subnational coverage estimates (mean, lower, upper) were incorrectly combined using a population-weighted average.</t>
+  </si>
+  <si>
+    <t>This should be corrected</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,6 +701,26 @@
         <v>34</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>44204</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>